<commit_message>
Fifth commit - Various updates including highlighting the max Total SAT Score
</commit_message>
<xml_diff>
--- a/sat_condensed.xlsx
+++ b/sat_condensed.xlsx
@@ -29,12 +29,17 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +60,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -26342,7 +26348,7 @@
       <c r="G632" t="n">
         <v>723.8</v>
       </c>
-      <c r="H632" t="n">
+      <c r="H632" s="2" t="n">
         <v>1440</v>
       </c>
       <c r="I632" t="inlineStr">

</xml_diff>

<commit_message>
Total SAT Score per County bar chart developed via Plotly
</commit_message>
<xml_diff>
--- a/sat_condensed.xlsx
+++ b/sat_condensed.xlsx
@@ -29,17 +29,12 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00008000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -60,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -26348,7 +26342,7 @@
       <c r="G632" t="n">
         <v>723.8</v>
       </c>
-      <c r="H632" s="2" t="n">
+      <c r="H632" t="n">
         <v>1440</v>
       </c>
       <c r="I632" t="inlineStr">

</xml_diff>